<commit_message>
Add a ton more content.  Thank you long flight to the midwest
</commit_message>
<xml_diff>
--- a/References/intro-to-investing.xlsx
+++ b/References/intro-to-investing.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpowers/Dropbox/Personal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpowers/code/College-Grads/References/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{903B2042-1003-844F-8F48-4DA853D0D510}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9508467-2C63-D94A-9651-BBDD99CF3329}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="1480" windowWidth="19360" windowHeight="19600" activeTab="1" xr2:uid="{3D93330D-5F01-FF4C-B97F-676D806834AD}"/>
+    <workbookView xWindow="4260" yWindow="1820" windowWidth="23420" windowHeight="21960" activeTab="2" xr2:uid="{3D93330D-5F01-FF4C-B97F-676D806834AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Investment terms" sheetId="1" r:id="rId1"/>
-    <sheet name="Mortage return" sheetId="2" r:id="rId2"/>
+    <sheet name="Taxes" sheetId="3" r:id="rId2"/>
+    <sheet name="Mortage return" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Rate of return</t>
   </si>
@@ -77,6 +78,33 @@
   </si>
   <si>
     <t>For the whole year</t>
+  </si>
+  <si>
+    <t>Number of Shares</t>
+  </si>
+  <si>
+    <t>Price per share</t>
+  </si>
+  <si>
+    <t>Recognized W2 Income</t>
+  </si>
+  <si>
+    <t>Cost basis reported to IRS</t>
+  </si>
+  <si>
+    <t>Theoretical tax rate</t>
+  </si>
+  <si>
+    <t>Total value at sale</t>
+  </si>
+  <si>
+    <t>Value minus reported cost basis</t>
+  </si>
+  <si>
+    <t>Value minus W2 income</t>
+  </si>
+  <si>
+    <t>Taxes owed</t>
   </si>
 </sst>
 </file>
@@ -138,7 +166,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
@@ -147,6 +175,9 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -466,7 +497,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -576,11 +607,110 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1355A292-75C2-0948-B95B-097CA5440595}">
+  <dimension ref="A2:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="23.83203125" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" ht="17">
+      <c r="A2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17">
+      <c r="A3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17">
+      <c r="A4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="34">
+      <c r="A5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17">
+      <c r="A6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17">
+      <c r="A8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <f>B2*B3</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="34">
+      <c r="A9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <f>B8-B5</f>
+        <v>100</v>
+      </c>
+      <c r="C9">
+        <f>B9*B6</f>
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="34">
+      <c r="A10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <f>B8-B4</f>
+        <v>-10</v>
+      </c>
+      <c r="C10">
+        <f>B10*B6</f>
+        <v>-2.5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5234CCC-56F8-3F41-A0C1-660B6027517F}">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>